<commit_message>
Resubmission of project 1 for the Udacity Data Analyst nanodegree
</commit_message>
<xml_diff>
--- a/stroopdata.xlsx
+++ b/stroopdata.xlsx
@@ -9,11 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="stroopdata" sheetId="1" r:id="rId1"/>
-    <sheet name="Fig 2A (ful data)" sheetId="3" r:id="rId2"/>
+    <sheet name="Fig 2A (full data)" sheetId="3" r:id="rId2"/>
     <sheet name="Fig 2B (Censored data)" sheetId="4" r:id="rId3"/>
     <sheet name="Fig 1 (histograms)" sheetId="5" r:id="rId4"/>
   </sheets>
@@ -759,10 +759,10 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
                   <c:pt idx="0">
-                    <c:v>3.4844157127666331</c:v>
+                    <c:v>3.5593579576451955</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>4.6960551345133172</c:v>
+                    <c:v>4.7970571224691376</c:v>
                   </c:pt>
                   <c:pt idx="2">
                     <c:v>4.8648269103590538</c:v>
@@ -777,10 +777,10 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
                   <c:pt idx="0">
-                    <c:v>3.4844157127666331</c:v>
+                    <c:v>3.5593579576451955</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>4.6960551345133172</c:v>
+                    <c:v>4.7970571224691376</c:v>
                   </c:pt>
                   <c:pt idx="2">
                     <c:v>4.8648269103590538</c:v>
@@ -893,11 +893,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="381541136"/>
-        <c:axId val="381541528"/>
+        <c:axId val="307382992"/>
+        <c:axId val="307383384"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="381541136"/>
+        <c:axId val="307382992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -954,7 +954,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="381541528"/>
+        <c:crossAx val="307383384"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -962,7 +962,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="381541528"/>
+        <c:axId val="307383384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1019,7 +1019,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="381541136"/>
+        <c:crossAx val="307382992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1126,88 +1126,88 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Fig 2A (ful data)'!$F$2:$F$26</c:f>
+              <c:f>'Fig 2A (full data)'!$F$2:$F$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="25"/>
                 <c:pt idx="0">
-                  <c:v>-1.2629754229900199</c:v>
+                  <c:v>-1.2363834885592544</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-1.2113207737064262</c:v>
+                  <c:v>-1.1858164273805361</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-1.1794040798401417</c:v>
+                  <c:v>-1.1545717391725481</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-1.1607160156684349</c:v>
+                  <c:v>-1.1362771519981334</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-0.96984578721808545</c:v>
+                  <c:v>-0.94942569422799317</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-0.95829698351646875</c:v>
+                  <c:v>-0.93812005046852331</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-0.88984407430325185</c:v>
+                  <c:v>-0.8711084165487587</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-0.59041509105770862</c:v>
+                  <c:v>-0.57798390743960504</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-0.39555527587407241</c:v>
+                  <c:v>-0.38722686364346504</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-0.27733752161934583</c:v>
+                  <c:v>-0.27149818297835082</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-0.19061650473266309</c:v>
+                  <c:v>-0.18660307620269817</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-0.16079959335758101</c:v>
+                  <c:v>-0.15741395958734072</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3.5530069569897176E-2</c:v>
+                  <c:v>3.4781984323640797E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>9.285413157973782E-2</c:v>
+                  <c:v>9.0899088802461572E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.14177906362476753</c:v>
+                  <c:v>0.13879390691076002</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.38325405011310881</c:v>
+                  <c:v>0.37518464006330327</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.40215209253393552</c:v>
+                  <c:v>0.39368478439698057</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.43322887340373978</c:v>
+                  <c:v>0.42410724396791688</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.62682881909265298</c:v>
+                  <c:v>0.61363094480847735</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.71312987948109574</c:v>
+                  <c:v>0.69811493726560436</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.77381359347686118</c:v>
+                  <c:v>0.7575209562926345</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.80573028734314656</c:v>
+                  <c:v>0.78876564450062303</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1.9087460299720673</c:v>
+                  <c:v>1.8685574021095899</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2.9300802336931908</c:v>
+                  <c:v>2.8683874247652161</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Fig 2A (ful data)'!$E$2:$E$26</c:f>
+              <c:f>'Fig 2A (full data)'!$E$2:$E$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="25"/>
@@ -1324,7 +1324,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Fig 2A (ful data)'!$E$2:$E$26</c:f>
+              <c:f>'Fig 2A (full data)'!$E$2:$E$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="25"/>
@@ -1408,7 +1408,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Fig 2A (ful data)'!$E$2:$E$26</c:f>
+              <c:f>'Fig 2A (full data)'!$E$2:$E$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="25"/>
@@ -1500,11 +1500,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="381542312"/>
-        <c:axId val="381540352"/>
+        <c:axId val="307384168"/>
+        <c:axId val="307389656"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="381542312"/>
+        <c:axId val="307384168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="-2.5"/>
@@ -1551,6 +1551,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1617,12 +1618,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="381540352"/>
+        <c:crossAx val="307389656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="381540352"/>
+        <c:axId val="307389656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2.5"/>
@@ -1670,6 +1671,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1736,7 +1738,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="381542312"/>
+        <c:crossAx val="307384168"/>
         <c:crossesAt val="-2.5"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.75000000000000011"/>
@@ -1916,70 +1918,70 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="22"/>
                 <c:pt idx="0">
-                  <c:v>-1.5443689284054838</c:v>
+                  <c:v>-1.5088614480568745</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-1.4678860572702401</c:v>
+                  <c:v>-1.4341370389017252</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-1.4206283482761071</c:v>
+                  <c:v>-1.3879658592611461</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-1.3929577160361202</c:v>
+                  <c:v>-1.360931418550543</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-1.110344180011992</c:v>
+                  <c:v>-1.0848156139894456</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-1.0932443510996404</c:v>
+                  <c:v>-1.0681089371458143</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-0.99188900154643211</c:v>
+                  <c:v>-0.96908390712720238</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-0.54853707374620353</c:v>
+                  <c:v>-0.53592534023597516</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-0.26001632409780673</c:v>
+                  <c:v>-0.25403813821980359</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-8.4976257231377791E-2</c:v>
+                  <c:v>-8.3022518893183697E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4.3427912601367476E-2</c:v>
+                  <c:v>4.2429436314444069E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>8.7576561793255472E-2</c:v>
+                  <c:v>8.5563038347090711E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.3782736533032241</c:v>
+                  <c:v>0.36957654468881512</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.46315098590452958</c:v>
+                  <c:v>0.45250241338538194</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.53559207929685382</c:v>
+                  <c:v>0.52327797165021861</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.89313395655510275</c:v>
+                  <c:v>0.87259939656249874</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.92111549477531351</c:v>
+                  <c:v>0.89993759503389448</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.96712957984854953</c:v>
+                  <c:v>0.94489374363130152</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.2537848936155971</c:v>
+                  <c:v>1.2249583990827115</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1.3815672514878943</c:v>
+                  <c:v>1.3498028387687537</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1.4714190797727926</c:v>
+                  <c:v>1.437588831638013</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1.5186767887669268</c:v>
+                  <c:v>1.4837600112785931</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2164,11 +2166,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="381538392"/>
-        <c:axId val="381543880"/>
+        <c:axId val="307388872"/>
+        <c:axId val="307388088"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="381538392"/>
+        <c:axId val="307388872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2.25"/>
@@ -2202,6 +2204,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2268,13 +2271,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="381543880"/>
+        <c:crossAx val="307388088"/>
         <c:crossesAt val="-2.25"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.75000000000000011"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="381543880"/>
+        <c:axId val="307388088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="-2.25"/>
@@ -2321,6 +2324,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2386,7 +2390,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="381538392"/>
+        <c:crossAx val="307388872"/>
         <c:crossesAt val="-2.25"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.75000000000000011"/>
@@ -2800,11 +2804,11 @@
         </c:dLbls>
         <c:gapWidth val="80"/>
         <c:overlap val="25"/>
-        <c:axId val="381538000"/>
-        <c:axId val="381539176"/>
+        <c:axId val="307385736"/>
+        <c:axId val="307384952"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="381538000"/>
+        <c:axId val="307385736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2836,7 +2840,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2903,7 +2906,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="381539176"/>
+        <c:crossAx val="307384952"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2911,7 +2914,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="381539176"/>
+        <c:axId val="307384952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2957,7 +2960,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3018,7 +3020,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="381538000"/>
+        <c:crossAx val="307385736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3032,7 +3034,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5732,8 +5733,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E25"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="J34" sqref="J34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5808,7 +5809,7 @@
       </c>
       <c r="N2">
         <f>B33</f>
-        <v>3.4844157127666331</v>
+        <v>3.5593579576451955</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -5858,7 +5859,7 @@
       </c>
       <c r="N3">
         <f>E33</f>
-        <v>4.6960551345133172</v>
+        <v>4.7970571224691376</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -6792,7 +6793,7 @@
       </c>
       <c r="L27">
         <f>H27/J33</f>
-        <v>8.020706944109957</v>
+        <v>7.8518310425969933</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
@@ -6839,12 +6840,12 @@
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B31">
-        <f>SUM(D2:D25)/24</f>
-        <v>12.141152859375003</v>
+        <f>SUM(D2:D25)/23</f>
+        <v>12.669029070652176</v>
       </c>
       <c r="E31">
-        <f>SUM(G2:G25)/24</f>
-        <v>22.052933826388891</v>
+        <f>SUM(G2:G25)/23</f>
+        <v>23.011757036231884</v>
       </c>
       <c r="H31">
         <f>SUM(J2:J25)/23</f>
@@ -6868,19 +6869,19 @@
     <row r="33" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B33">
         <f>SQRT(B31)</f>
-        <v>3.4844157127666331</v>
+        <v>3.5593579576451955</v>
       </c>
       <c r="E33">
         <f>SQRT(E31)</f>
-        <v>4.6960551345133172</v>
+        <v>4.7970571224691376</v>
       </c>
       <c r="H33">
         <f>SQRT(H31)</f>
         <v>4.8648269103590538</v>
       </c>
       <c r="J33">
-        <f>H33/SQRT(24)</f>
-        <v>0.99302863477834025</v>
+        <f>H33/SQRT(23)</f>
+        <v>1.0143865327026076</v>
       </c>
     </row>
   </sheetData>
@@ -6893,8 +6894,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N20" sqref="N20"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6942,8 +6943,8 @@
         <v>-2</v>
       </c>
       <c r="F2">
-        <f>(Table1[[#This Row],[Data]]-AVERAGE(Table1[Data]))/SQRT(SUM($I$2:$I$25)/24)</f>
-        <v>-1.2629754229900199</v>
+        <f>(Table1[[#This Row],[Data]]-AVERAGE(Table1[Data]))/SQRT(SUM($I$2:$I$25)/23)</f>
+        <v>-1.2363834885592544</v>
       </c>
       <c r="H2">
         <f>Table1[[#This Row],[Data]]-AVERAGE($A$2:$A$26)</f>
@@ -6974,8 +6975,8 @@
         <v>-1.826087</v>
       </c>
       <c r="F3">
-        <f>(Table1[[#This Row],[Data]]-AVERAGE(Table1[Data]))/SQRT(SUM($I$2:$I$25)/24)</f>
-        <v>-1.2113207737064262</v>
+        <f>(Table1[[#This Row],[Data]]-AVERAGE(Table1[Data]))/SQRT(SUM($I$2:$I$25)/23)</f>
+        <v>-1.1858164273805361</v>
       </c>
       <c r="H3">
         <f>Table1[[#This Row],[Data]]-AVERAGE($A$2:$A$26)</f>
@@ -7006,8 +7007,8 @@
         <v>-1.652174</v>
       </c>
       <c r="F4">
-        <f>(Table1[[#This Row],[Data]]-AVERAGE(Table1[Data]))/SQRT(SUM($I$2:$I$25)/24)</f>
-        <v>-1.1794040798401417</v>
+        <f>(Table1[[#This Row],[Data]]-AVERAGE(Table1[Data]))/SQRT(SUM($I$2:$I$25)/23)</f>
+        <v>-1.1545717391725481</v>
       </c>
       <c r="H4">
         <f>Table1[[#This Row],[Data]]-AVERAGE($A$2:$A$26)</f>
@@ -7038,8 +7039,8 @@
         <v>-1.478261</v>
       </c>
       <c r="F5">
-        <f>(Table1[[#This Row],[Data]]-AVERAGE(Table1[Data]))/SQRT(SUM($I$2:$I$25)/24)</f>
-        <v>-1.1607160156684349</v>
+        <f>(Table1[[#This Row],[Data]]-AVERAGE(Table1[Data]))/SQRT(SUM($I$2:$I$25)/23)</f>
+        <v>-1.1362771519981334</v>
       </c>
       <c r="H5">
         <f>Table1[[#This Row],[Data]]-AVERAGE($A$2:$A$26)</f>
@@ -7070,8 +7071,8 @@
         <v>-1.3043480000000001</v>
       </c>
       <c r="F6">
-        <f>(Table1[[#This Row],[Data]]-AVERAGE(Table1[Data]))/SQRT(SUM($I$2:$I$25)/24)</f>
-        <v>-0.96984578721808545</v>
+        <f>(Table1[[#This Row],[Data]]-AVERAGE(Table1[Data]))/SQRT(SUM($I$2:$I$25)/23)</f>
+        <v>-0.94942569422799317</v>
       </c>
       <c r="H6">
         <f>Table1[[#This Row],[Data]]-AVERAGE($A$2:$A$26)</f>
@@ -7102,8 +7103,8 @@
         <v>-1.1304350000000001</v>
       </c>
       <c r="F7">
-        <f>(Table1[[#This Row],[Data]]-AVERAGE(Table1[Data]))/SQRT(SUM($I$2:$I$25)/24)</f>
-        <v>-0.95829698351646875</v>
+        <f>(Table1[[#This Row],[Data]]-AVERAGE(Table1[Data]))/SQRT(SUM($I$2:$I$25)/23)</f>
+        <v>-0.93812005046852331</v>
       </c>
       <c r="H7">
         <f>Table1[[#This Row],[Data]]-AVERAGE($A$2:$A$26)</f>
@@ -7134,8 +7135,8 @@
         <v>-0.95652200000000009</v>
       </c>
       <c r="F8">
-        <f>(Table1[[#This Row],[Data]]-AVERAGE(Table1[Data]))/SQRT(SUM($I$2:$I$25)/24)</f>
-        <v>-0.88984407430325185</v>
+        <f>(Table1[[#This Row],[Data]]-AVERAGE(Table1[Data]))/SQRT(SUM($I$2:$I$25)/23)</f>
+        <v>-0.8711084165487587</v>
       </c>
       <c r="H8">
         <f>Table1[[#This Row],[Data]]-AVERAGE($A$2:$A$26)</f>
@@ -7166,8 +7167,8 @@
         <v>-0.78260900000000011</v>
       </c>
       <c r="F9">
-        <f>(Table1[[#This Row],[Data]]-AVERAGE(Table1[Data]))/SQRT(SUM($I$2:$I$25)/24)</f>
-        <v>-0.59041509105770862</v>
+        <f>(Table1[[#This Row],[Data]]-AVERAGE(Table1[Data]))/SQRT(SUM($I$2:$I$25)/23)</f>
+        <v>-0.57798390743960504</v>
       </c>
       <c r="H9">
         <f>Table1[[#This Row],[Data]]-AVERAGE($A$2:$A$26)</f>
@@ -7198,8 +7199,8 @@
         <v>-0.60869600000000013</v>
       </c>
       <c r="F10">
-        <f>(Table1[[#This Row],[Data]]-AVERAGE(Table1[Data]))/SQRT(SUM($I$2:$I$25)/24)</f>
-        <v>-0.39555527587407241</v>
+        <f>(Table1[[#This Row],[Data]]-AVERAGE(Table1[Data]))/SQRT(SUM($I$2:$I$25)/23)</f>
+        <v>-0.38722686364346504</v>
       </c>
       <c r="H10">
         <f>Table1[[#This Row],[Data]]-AVERAGE($A$2:$A$26)</f>
@@ -7230,8 +7231,8 @@
         <v>-0.43478300000000014</v>
       </c>
       <c r="F11">
-        <f>(Table1[[#This Row],[Data]]-AVERAGE(Table1[Data]))/SQRT(SUM($I$2:$I$25)/24)</f>
-        <v>-0.27733752161934583</v>
+        <f>(Table1[[#This Row],[Data]]-AVERAGE(Table1[Data]))/SQRT(SUM($I$2:$I$25)/23)</f>
+        <v>-0.27149818297835082</v>
       </c>
       <c r="H11">
         <f>Table1[[#This Row],[Data]]-AVERAGE($A$2:$A$26)</f>
@@ -7262,8 +7263,8 @@
         <v>-0.26087000000000016</v>
       </c>
       <c r="F12">
-        <f>(Table1[[#This Row],[Data]]-AVERAGE(Table1[Data]))/SQRT(SUM($I$2:$I$25)/24)</f>
-        <v>-0.19061650473266309</v>
+        <f>(Table1[[#This Row],[Data]]-AVERAGE(Table1[Data]))/SQRT(SUM($I$2:$I$25)/23)</f>
+        <v>-0.18660307620269817</v>
       </c>
       <c r="H12">
         <f>Table1[[#This Row],[Data]]-AVERAGE($A$2:$A$26)</f>
@@ -7294,8 +7295,8 @@
         <v>-8.6957000000000145E-2</v>
       </c>
       <c r="F13">
-        <f>(Table1[[#This Row],[Data]]-AVERAGE(Table1[Data]))/SQRT(SUM($I$2:$I$25)/24)</f>
-        <v>-0.16079959335758101</v>
+        <f>(Table1[[#This Row],[Data]]-AVERAGE(Table1[Data]))/SQRT(SUM($I$2:$I$25)/23)</f>
+        <v>-0.15741395958734072</v>
       </c>
       <c r="H13">
         <f>Table1[[#This Row],[Data]]-AVERAGE($A$2:$A$26)</f>
@@ -7326,8 +7327,8 @@
         <v>8.6955999999999867E-2</v>
       </c>
       <c r="F14">
-        <f>(Table1[[#This Row],[Data]]-AVERAGE(Table1[Data]))/SQRT(SUM($I$2:$I$25)/24)</f>
-        <v>3.5530069569897176E-2</v>
+        <f>(Table1[[#This Row],[Data]]-AVERAGE(Table1[Data]))/SQRT(SUM($I$2:$I$25)/23)</f>
+        <v>3.4781984323640797E-2</v>
       </c>
       <c r="H14">
         <f>Table1[[#This Row],[Data]]-AVERAGE($A$2:$A$26)</f>
@@ -7358,8 +7359,8 @@
         <v>0.26086899999999991</v>
       </c>
       <c r="F15">
-        <f>(Table1[[#This Row],[Data]]-AVERAGE(Table1[Data]))/SQRT(SUM($I$2:$I$25)/24)</f>
-        <v>9.285413157973782E-2</v>
+        <f>(Table1[[#This Row],[Data]]-AVERAGE(Table1[Data]))/SQRT(SUM($I$2:$I$25)/23)</f>
+        <v>9.0899088802461572E-2</v>
       </c>
       <c r="H15">
         <f>Table1[[#This Row],[Data]]-AVERAGE($A$2:$A$26)</f>
@@ -7390,8 +7391,8 @@
         <v>0.43478199999999989</v>
       </c>
       <c r="F16">
-        <f>(Table1[[#This Row],[Data]]-AVERAGE(Table1[Data]))/SQRT(SUM($I$2:$I$25)/24)</f>
-        <v>0.14177906362476753</v>
+        <f>(Table1[[#This Row],[Data]]-AVERAGE(Table1[Data]))/SQRT(SUM($I$2:$I$25)/23)</f>
+        <v>0.13879390691076002</v>
       </c>
       <c r="H16">
         <f>Table1[[#This Row],[Data]]-AVERAGE($A$2:$A$26)</f>
@@ -7422,8 +7423,8 @@
         <v>0.60869499999999988</v>
       </c>
       <c r="F17">
-        <f>(Table1[[#This Row],[Data]]-AVERAGE(Table1[Data]))/SQRT(SUM($I$2:$I$25)/24)</f>
-        <v>0.38325405011310881</v>
+        <f>(Table1[[#This Row],[Data]]-AVERAGE(Table1[Data]))/SQRT(SUM($I$2:$I$25)/23)</f>
+        <v>0.37518464006330327</v>
       </c>
       <c r="H17">
         <f>Table1[[#This Row],[Data]]-AVERAGE($A$2:$A$26)</f>
@@ -7454,8 +7455,8 @@
         <v>0.78260799999999986</v>
       </c>
       <c r="F18">
-        <f>(Table1[[#This Row],[Data]]-AVERAGE(Table1[Data]))/SQRT(SUM($I$2:$I$25)/24)</f>
-        <v>0.40215209253393552</v>
+        <f>(Table1[[#This Row],[Data]]-AVERAGE(Table1[Data]))/SQRT(SUM($I$2:$I$25)/23)</f>
+        <v>0.39368478439698057</v>
       </c>
       <c r="H18">
         <f>Table1[[#This Row],[Data]]-AVERAGE($A$2:$A$26)</f>
@@ -7486,8 +7487,8 @@
         <v>0.95652099999999984</v>
       </c>
       <c r="F19">
-        <f>(Table1[[#This Row],[Data]]-AVERAGE(Table1[Data]))/SQRT(SUM($I$2:$I$25)/24)</f>
-        <v>0.43322887340373978</v>
+        <f>(Table1[[#This Row],[Data]]-AVERAGE(Table1[Data]))/SQRT(SUM($I$2:$I$25)/23)</f>
+        <v>0.42410724396791688</v>
       </c>
       <c r="H19">
         <f>Table1[[#This Row],[Data]]-AVERAGE($A$2:$A$26)</f>
@@ -7518,8 +7519,8 @@
         <v>1.1304339999999999</v>
       </c>
       <c r="F20">
-        <f>(Table1[[#This Row],[Data]]-AVERAGE(Table1[Data]))/SQRT(SUM($I$2:$I$25)/24)</f>
-        <v>0.62682881909265298</v>
+        <f>(Table1[[#This Row],[Data]]-AVERAGE(Table1[Data]))/SQRT(SUM($I$2:$I$25)/23)</f>
+        <v>0.61363094480847735</v>
       </c>
       <c r="H20">
         <f>Table1[[#This Row],[Data]]-AVERAGE($A$2:$A$26)</f>
@@ -7550,8 +7551,8 @@
         <v>1.3043469999999999</v>
       </c>
       <c r="F21">
-        <f>(Table1[[#This Row],[Data]]-AVERAGE(Table1[Data]))/SQRT(SUM($I$2:$I$25)/24)</f>
-        <v>0.71312987948109574</v>
+        <f>(Table1[[#This Row],[Data]]-AVERAGE(Table1[Data]))/SQRT(SUM($I$2:$I$25)/23)</f>
+        <v>0.69811493726560436</v>
       </c>
       <c r="H21">
         <f>Table1[[#This Row],[Data]]-AVERAGE($A$2:$A$26)</f>
@@ -7582,8 +7583,8 @@
         <v>1.4782599999999999</v>
       </c>
       <c r="F22">
-        <f>(Table1[[#This Row],[Data]]-AVERAGE(Table1[Data]))/SQRT(SUM($I$2:$I$25)/24)</f>
-        <v>0.77381359347686118</v>
+        <f>(Table1[[#This Row],[Data]]-AVERAGE(Table1[Data]))/SQRT(SUM($I$2:$I$25)/23)</f>
+        <v>0.7575209562926345</v>
       </c>
       <c r="H22">
         <f>Table1[[#This Row],[Data]]-AVERAGE($A$2:$A$26)</f>
@@ -7614,8 +7615,8 @@
         <v>1.6521729999999999</v>
       </c>
       <c r="F23">
-        <f>(Table1[[#This Row],[Data]]-AVERAGE(Table1[Data]))/SQRT(SUM($I$2:$I$25)/24)</f>
-        <v>0.80573028734314656</v>
+        <f>(Table1[[#This Row],[Data]]-AVERAGE(Table1[Data]))/SQRT(SUM($I$2:$I$25)/23)</f>
+        <v>0.78876564450062303</v>
       </c>
       <c r="H23">
         <f>Table1[[#This Row],[Data]]-AVERAGE($A$2:$A$26)</f>
@@ -7646,8 +7647,8 @@
         <v>1.8260859999999999</v>
       </c>
       <c r="F24">
-        <f>(Table1[[#This Row],[Data]]-AVERAGE(Table1[Data]))/SQRT(SUM($I$2:$I$25)/24)</f>
-        <v>1.9087460299720673</v>
+        <f>(Table1[[#This Row],[Data]]-AVERAGE(Table1[Data]))/SQRT(SUM($I$2:$I$25)/23)</f>
+        <v>1.8685574021095899</v>
       </c>
       <c r="H24">
         <f>Table1[[#This Row],[Data]]-AVERAGE($A$2:$A$26)</f>
@@ -7678,8 +7679,8 @@
         <v>1.9999989999999999</v>
       </c>
       <c r="F25">
-        <f>(Table1[[#This Row],[Data]]-AVERAGE(Table1[Data]))/SQRT(SUM($I$2:$I$25)/24)</f>
-        <v>2.9300802336931908</v>
+        <f>(Table1[[#This Row],[Data]]-AVERAGE(Table1[Data]))/SQRT(SUM($I$2:$I$25)/23)</f>
+        <v>2.8683874247652161</v>
       </c>
       <c r="H25">
         <f>Table1[[#This Row],[Data]]-AVERAGE($A$2:$A$26)</f>
@@ -7712,8 +7713,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7759,7 +7760,7 @@
       </c>
       <c r="F2" s="7">
         <f>(A2-AVERAGE($A$2:$A$23))/$H$26</f>
-        <v>-1.5443689284054838</v>
+        <v>-1.5088614480568745</v>
       </c>
       <c r="G2">
         <f>A2-AVERAGE(A2:A23)</f>
@@ -7791,7 +7792,7 @@
       </c>
       <c r="F3" s="7">
         <f t="shared" ref="F3:F23" si="2">(A3-AVERAGE($A$2:$A$23))/$H$26</f>
-        <v>-1.4678860572702401</v>
+        <v>-1.4341370389017252</v>
       </c>
       <c r="G3">
         <f t="shared" ref="G3:G23" si="3">A3-AVERAGE(A3:A24)</f>
@@ -7823,7 +7824,7 @@
       </c>
       <c r="F4" s="7">
         <f t="shared" si="2"/>
-        <v>-1.4206283482761071</v>
+        <v>-1.3879658592611461</v>
       </c>
       <c r="G4">
         <f t="shared" si="3"/>
@@ -7855,7 +7856,7 @@
       </c>
       <c r="F5" s="7">
         <f t="shared" si="2"/>
-        <v>-1.3929577160361202</v>
+        <v>-1.360931418550543</v>
       </c>
       <c r="G5">
         <f t="shared" si="3"/>
@@ -7887,7 +7888,7 @@
       </c>
       <c r="F6" s="7">
         <f t="shared" si="2"/>
-        <v>-1.110344180011992</v>
+        <v>-1.0848156139894456</v>
       </c>
       <c r="G6">
         <f t="shared" si="3"/>
@@ -7919,7 +7920,7 @@
       </c>
       <c r="F7" s="7">
         <f t="shared" si="2"/>
-        <v>-1.0932443510996404</v>
+        <v>-1.0681089371458143</v>
       </c>
       <c r="G7">
         <f t="shared" si="3"/>
@@ -7951,7 +7952,7 @@
       </c>
       <c r="F8" s="7">
         <f t="shared" si="2"/>
-        <v>-0.99188900154643211</v>
+        <v>-0.96908390712720238</v>
       </c>
       <c r="G8">
         <f t="shared" si="3"/>
@@ -7983,7 +7984,7 @@
       </c>
       <c r="F9" s="7">
         <f t="shared" si="2"/>
-        <v>-0.54853707374620353</v>
+        <v>-0.53592534023597516</v>
       </c>
       <c r="G9">
         <f t="shared" si="3"/>
@@ -8015,7 +8016,7 @@
       </c>
       <c r="F10" s="7">
         <f t="shared" si="2"/>
-        <v>-0.26001632409780673</v>
+        <v>-0.25403813821980359</v>
       </c>
       <c r="G10">
         <f t="shared" si="3"/>
@@ -8047,7 +8048,7 @@
       </c>
       <c r="F11" s="7">
         <f t="shared" si="2"/>
-        <v>-8.4976257231377791E-2</v>
+        <v>-8.3022518893183697E-2</v>
       </c>
       <c r="G11">
         <f t="shared" si="3"/>
@@ -8079,7 +8080,7 @@
       </c>
       <c r="F12" s="7">
         <f t="shared" si="2"/>
-        <v>4.3427912601367476E-2</v>
+        <v>4.2429436314444069E-2</v>
       </c>
       <c r="G12">
         <f t="shared" si="3"/>
@@ -8111,7 +8112,7 @@
       </c>
       <c r="F13" s="7">
         <f t="shared" si="2"/>
-        <v>8.7576561793255472E-2</v>
+        <v>8.5563038347090711E-2</v>
       </c>
       <c r="G13">
         <f t="shared" si="3"/>
@@ -8143,7 +8144,7 @@
       </c>
       <c r="F14" s="7">
         <f t="shared" si="2"/>
-        <v>0.3782736533032241</v>
+        <v>0.36957654468881512</v>
       </c>
       <c r="G14">
         <f t="shared" si="3"/>
@@ -8175,7 +8176,7 @@
       </c>
       <c r="F15" s="7">
         <f t="shared" si="2"/>
-        <v>0.46315098590452958</v>
+        <v>0.45250241338538194</v>
       </c>
       <c r="G15">
         <f t="shared" si="3"/>
@@ -8207,7 +8208,7 @@
       </c>
       <c r="F16" s="7">
         <f t="shared" si="2"/>
-        <v>0.53559207929685382</v>
+        <v>0.52327797165021861</v>
       </c>
       <c r="G16">
         <f t="shared" si="3"/>
@@ -8239,7 +8240,7 @@
       </c>
       <c r="F17" s="7">
         <f t="shared" si="2"/>
-        <v>0.89313395655510275</v>
+        <v>0.87259939656249874</v>
       </c>
       <c r="G17">
         <f t="shared" si="3"/>
@@ -8271,7 +8272,7 @@
       </c>
       <c r="F18" s="7">
         <f t="shared" si="2"/>
-        <v>0.92111549477531351</v>
+        <v>0.89993759503389448</v>
       </c>
       <c r="G18">
         <f t="shared" si="3"/>
@@ -8303,7 +8304,7 @@
       </c>
       <c r="F19" s="7">
         <f t="shared" si="2"/>
-        <v>0.96712957984854953</v>
+        <v>0.94489374363130152</v>
       </c>
       <c r="G19">
         <f t="shared" si="3"/>
@@ -8335,7 +8336,7 @@
       </c>
       <c r="F20" s="7">
         <f t="shared" si="2"/>
-        <v>1.2537848936155971</v>
+        <v>1.2249583990827115</v>
       </c>
       <c r="G20">
         <f t="shared" si="3"/>
@@ -8367,7 +8368,7 @@
       </c>
       <c r="F21" s="7">
         <f t="shared" si="2"/>
-        <v>1.3815672514878943</v>
+        <v>1.3498028387687537</v>
       </c>
       <c r="G21">
         <f t="shared" si="3"/>
@@ -8399,7 +8400,7 @@
       </c>
       <c r="F22" s="7">
         <f t="shared" si="2"/>
-        <v>1.4714190797727926</v>
+        <v>1.437588831638013</v>
       </c>
       <c r="G22">
         <f t="shared" si="3"/>
@@ -8431,7 +8432,7 @@
       </c>
       <c r="F23" s="7">
         <f t="shared" si="2"/>
-        <v>1.5186767887669268</v>
+        <v>1.4837600112785931</v>
       </c>
       <c r="G23">
         <f t="shared" si="3"/>
@@ -8450,14 +8451,14 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H25">
-        <f>H24/22</f>
-        <v>10.345270448749163</v>
+        <f>H24/21</f>
+        <v>10.837902374880077</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H26">
         <f>SQRT(H25)</f>
-        <v>3.2164064495565796</v>
+        <v>3.2920969570898237</v>
       </c>
     </row>
   </sheetData>

</xml_diff>